<commit_message>
Densidad de frecuencia espectral_ejemplo
</commit_message>
<xml_diff>
--- a/Angulos.xlsx
+++ b/Angulos.xlsx
@@ -8,19 +8,35 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://correoitmedu-my.sharepoint.com/personal/juanrojas166633_correo_itm_edu_co/Documents/Maestria/Semestre_5/Resultados_Obje_2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0181778B-30E6-412A-B0BA-8DFE159D1B4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="136" documentId="8_{0181778B-30E6-412A-B0BA-8DFE159D1B4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{823792A5-0B8D-46C2-89A2-4CF8DACC068B}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{324C3B7B-0C75-45DC-B1CF-1FA0C0B0F17D}"/>
   </bookViews>
   <sheets>
     <sheet name="Angulos" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Angulos!$L$1:$L$28</definedName>
+  </definedNames>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="43">
   <si>
     <t>A</t>
   </si>
@@ -37,75 +53,24 @@
     <t>col 0</t>
   </si>
   <si>
-    <t>-63.43</t>
-  </si>
-  <si>
-    <t>-53.13</t>
-  </si>
-  <si>
-    <t>-45.0</t>
-  </si>
-  <si>
-    <t>-38.66</t>
-  </si>
-  <si>
     <t>col 1</t>
   </si>
   <si>
-    <t>-56.31</t>
-  </si>
-  <si>
-    <t>-36.87</t>
-  </si>
-  <si>
-    <t>-30.96</t>
-  </si>
-  <si>
     <t>col 2</t>
   </si>
   <si>
-    <t>-33.69</t>
-  </si>
-  <si>
-    <t>-26.57</t>
-  </si>
-  <si>
-    <t>-21.8</t>
-  </si>
-  <si>
     <t>col 3</t>
   </si>
   <si>
-    <t>-18.43</t>
-  </si>
-  <si>
-    <t>-14.04</t>
-  </si>
-  <si>
-    <t>-11.31</t>
-  </si>
-  <si>
     <t>col 4</t>
   </si>
   <si>
-    <t>0.0</t>
-  </si>
-  <si>
     <t>col 5</t>
   </si>
   <si>
     <t>26.57</t>
   </si>
   <si>
-    <t>18.43</t>
-  </si>
-  <si>
-    <t>14.04</t>
-  </si>
-  <si>
-    <t>11.31</t>
-  </si>
-  <si>
     <t>col 6</t>
   </si>
   <si>
@@ -115,9 +80,6 @@
     <t>33.69</t>
   </si>
   <si>
-    <t>21.8</t>
-  </si>
-  <si>
     <t>col 7</t>
   </si>
   <si>
@@ -127,9 +89,6 @@
     <t>36.87</t>
   </si>
   <si>
-    <t>30.96</t>
-  </si>
-  <si>
     <t>col 8</t>
   </si>
   <si>
@@ -139,10 +98,73 @@
     <t>53.13</t>
   </si>
   <si>
-    <t>38.66</t>
-  </si>
-  <si>
     <t>Ángulos (°)</t>
+  </si>
+  <si>
+    <t>90.0</t>
+  </si>
+  <si>
+    <t>135.0</t>
+  </si>
+  <si>
+    <t>116.57</t>
+  </si>
+  <si>
+    <t>75.96</t>
+  </si>
+  <si>
+    <t>120.96</t>
+  </si>
+  <si>
+    <t>111.8</t>
+  </si>
+  <si>
+    <t>101.31</t>
+  </si>
+  <si>
+    <t>78.69</t>
+  </si>
+  <si>
+    <t>68.2</t>
+  </si>
+  <si>
+    <t>59.04</t>
+  </si>
+  <si>
+    <t>51.34</t>
+  </si>
+  <si>
+    <t>126.87</t>
+  </si>
+  <si>
+    <t>104.04</t>
+  </si>
+  <si>
+    <t>123.69</t>
+  </si>
+  <si>
+    <t>143.13</t>
+  </si>
+  <si>
+    <t>108.43</t>
+  </si>
+  <si>
+    <t>71.57</t>
+  </si>
+  <si>
+    <t>153.43</t>
+  </si>
+  <si>
+    <t>146.31</t>
+  </si>
+  <si>
+    <t>128.66</t>
+  </si>
+  <si>
+    <t>Tomar más muestras</t>
+  </si>
+  <si>
+    <t>Muestras</t>
   </si>
 </sst>
 </file>
@@ -285,7 +307,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="36">
+  <fills count="50">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -467,12 +489,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -480,6 +496,96 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.749992370372631"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -659,17 +765,60 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="40" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="41" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="42" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="43" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="44" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="45" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="46" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="47" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="48" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="49" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1047,191 +1196,522 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACF10BC2-FB0C-4ECF-90D7-649E7AA759FE}">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:N28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:J6"/>
+      <selection activeCell="Q24" sqref="Q24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="7.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="5" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+      <c r="L1" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="M1" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="N1" s="17" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
+      <c r="B2" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="L2" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="M2" s="18">
+        <v>4</v>
+      </c>
+      <c r="N2" s="7">
+        <f>ABS(M2-4)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="6">
+        <v>12</v>
+      </c>
+      <c r="C3" s="16">
+        <v>12</v>
+      </c>
+      <c r="D3" s="3">
+        <v>6</v>
+      </c>
+      <c r="E3" s="4">
+        <v>6</v>
+      </c>
+      <c r="F3" s="3">
+        <v>3</v>
+      </c>
+      <c r="G3" s="4">
+        <v>6</v>
+      </c>
+      <c r="H3" s="3">
+        <v>6</v>
+      </c>
+      <c r="I3" s="16">
+        <v>12</v>
+      </c>
+      <c r="J3" s="6">
+        <v>12</v>
+      </c>
+      <c r="L3" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="M3" s="18">
+        <v>1</v>
+      </c>
+      <c r="N3" s="19">
+        <f>ABS(M3-4)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="5">
+        <v>12</v>
+      </c>
+      <c r="C4" s="3">
+        <v>3</v>
+      </c>
+      <c r="D4" s="14">
+        <v>12</v>
+      </c>
+      <c r="E4" s="15">
+        <v>12</v>
+      </c>
+      <c r="F4" s="3">
+        <v>3</v>
+      </c>
+      <c r="G4" s="15">
+        <v>12</v>
+      </c>
+      <c r="H4" s="14">
+        <v>12</v>
+      </c>
+      <c r="I4" s="3">
+        <v>3</v>
+      </c>
+      <c r="J4" s="5">
+        <v>12</v>
+      </c>
+      <c r="L4" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="M4" s="18">
+        <v>1</v>
+      </c>
+      <c r="N4" s="19">
+        <f>ABS(M4-4)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="3">
+        <v>3</v>
+      </c>
+      <c r="C5" s="13">
+        <v>12</v>
+      </c>
+      <c r="D5" s="4">
+        <v>6</v>
+      </c>
+      <c r="E5" s="12">
+        <v>12</v>
+      </c>
+      <c r="F5" s="3">
+        <v>3</v>
+      </c>
+      <c r="G5" s="12">
+        <v>12</v>
+      </c>
+      <c r="H5" s="4">
+        <v>6</v>
+      </c>
+      <c r="I5" s="13">
+        <v>12</v>
+      </c>
+      <c r="J5" s="3">
+        <v>3</v>
+      </c>
+      <c r="L5" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="M5" s="18">
+        <v>1</v>
+      </c>
+      <c r="N5" s="19">
+        <f>ABS(M5-4)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="8">
+        <v>12</v>
+      </c>
+      <c r="C6" s="9">
+        <v>12</v>
+      </c>
+      <c r="D6" s="10">
+        <v>12</v>
+      </c>
+      <c r="E6" s="11">
+        <v>12</v>
+      </c>
+      <c r="F6" s="3">
+        <v>3</v>
+      </c>
+      <c r="G6" s="11">
+        <v>12</v>
+      </c>
+      <c r="H6" s="10">
+        <v>12</v>
+      </c>
+      <c r="I6" s="9">
+        <v>12</v>
+      </c>
+      <c r="J6" s="8">
+        <v>12</v>
+      </c>
+      <c r="L6" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="M6" s="18">
+        <v>1</v>
+      </c>
+      <c r="N6" s="19">
+        <f>ABS(M6-4)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L7" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="M7" s="18">
+        <v>2</v>
+      </c>
+      <c r="N7" s="19">
+        <f>ABS(M7-4)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L8" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="M8" s="18">
+        <v>1</v>
+      </c>
+      <c r="N8" s="19">
+        <f>ABS(M8-4)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L9" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="M9" s="18">
+        <v>1</v>
+      </c>
+      <c r="N9" s="19">
+        <f>ABS(M9-4)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L10" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="M10" s="18">
+        <v>1</v>
+      </c>
+      <c r="N10" s="19">
+        <f>ABS(M10-4)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L11" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="M11" s="18">
+        <v>1</v>
+      </c>
+      <c r="N11" s="19">
+        <f>ABS(M11-4)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L12" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="M12" s="18">
+        <v>3</v>
+      </c>
+      <c r="N12" s="19">
+        <f>ABS(M12-4)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L13" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="M13" s="18">
+        <v>1</v>
+      </c>
+      <c r="N13" s="19">
+        <f>ABS(M13-4)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L14" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="M14" s="18">
+        <v>1</v>
+      </c>
+      <c r="N14" s="19">
+        <f>ABS(M14-4)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L15" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="M15" s="18">
+        <v>1</v>
+      </c>
+      <c r="N15" s="19">
+        <f>ABS(M15-4)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L16" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="M16" s="18">
+        <v>1</v>
+      </c>
+      <c r="N16" s="19">
+        <f>ABS(M16-4)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="L17" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="M17" s="18">
+        <v>1</v>
+      </c>
+      <c r="N17" s="19">
+        <f>ABS(M17-4)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="L18" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="M18" s="18">
+        <v>1</v>
+      </c>
+      <c r="N18" s="19">
+        <f>ABS(M18-4)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="L19" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="M19" s="18">
+        <v>3</v>
+      </c>
+      <c r="N19" s="19">
+        <f>ABS(M19-4)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="L20" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-      <c r="B2" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="G2" s="4" t="s">
+      <c r="M20" s="18">
+        <v>1</v>
+      </c>
+      <c r="N20" s="19">
+        <f>ABS(M20-4)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="L21" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="M21" s="18">
+        <v>1</v>
+      </c>
+      <c r="N21" s="19">
+        <f>ABS(M21-4)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="L22" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="M22" s="18">
+        <v>1</v>
+      </c>
+      <c r="N22" s="19">
+        <f>ABS(M22-4)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="L23" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="M23" s="18">
+        <v>1</v>
+      </c>
+      <c r="N23" s="19">
+        <f>ABS(M23-4)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="L24" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="H2" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="J2" s="4" t="s">
+      <c r="M24" s="18">
+        <v>2</v>
+      </c>
+      <c r="N24" s="19">
+        <f>ABS(M24-4)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="L25" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="M25" s="18">
+        <v>1</v>
+      </c>
+      <c r="N25" s="19">
+        <f>ABS(M25-4)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="L26" s="18" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="I3" s="5" t="s">
+      <c r="M26" s="18">
+        <v>1</v>
+      </c>
+      <c r="N26" s="19">
+        <f>ABS(M26-4)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="L27" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="J3" s="5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="I4" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="J4" s="5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="I5" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="J5" s="5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="G6" s="5" t="s">
+      <c r="M27" s="18">
+        <v>1</v>
+      </c>
+      <c r="N27" s="19">
+        <f>ABS(M27-4)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="L28" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="H6" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="I6" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="J6" s="5" t="s">
-        <v>39</v>
+      <c r="M28" s="18">
+        <v>1</v>
+      </c>
+      <c r="N28" s="19">
+        <f>ABS(M28-4)</f>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="L1:L28" xr:uid="{ACF10BC2-FB0C-4ECF-90D7-649E7AA759FE}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="L2:N28">
+      <sortCondition descending="1" ref="L1:L28"/>
+    </sortState>
+  </autoFilter>
   <mergeCells count="1">
     <mergeCell ref="B1:J1"/>
   </mergeCells>

</xml_diff>